<commit_message>
finding mean salary for business development position,
</commit_message>
<xml_diff>
--- a/indeed_job_searching_results.xlsx
+++ b/indeed_job_searching_results.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paxton615/Github_Personal/Indeed_Job_Search/Indeed_Job_Search/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23800" windowHeight="13420"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet5" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -820,12 +815,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -833,15 +828,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -891,14 +879,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -945,7 +925,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -977,27 +957,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1029,24 +991,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1222,19 +1166,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
-  <cols>
-    <col min="2" max="2" width="40.33203125" customWidth="1"/>
-    <col min="3" max="3" width="42.1640625" customWidth="1"/>
-    <col min="4" max="4" width="46" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
@@ -5168,8 +5105,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>